<commit_message>
- More tests filled in for _collects_nutrient_ratio_conflicts() - Last one failing at the moment.
</commit_message>
<xml_diff>
--- a/docs/flag_conflict_logic_table~v2.xlsx
+++ b/docs/flag_conflict_logic_table~v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.izzard\Dropbox\pydiet\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James.Izzard\Dropbox\pydiet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{6808ADB4-193F-4485-8AF5-471CCA1F3113}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ACDEBC-87E7-42CC-B03F-2A463B987F18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31440" yWindow="5100" windowWidth="40515" windowHeight="14790"/>
+    <workbookView xWindow="1860" yWindow="3210" windowWidth="43370" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
   <si>
     <t>Flag Type</t>
   </si>
@@ -135,12 +135,21 @@
   </si>
   <si>
     <t>test_none_to_none_returns_no_conflicts()</t>
+  </si>
+  <si>
+    <t>test_none_to_true_correctly_categorises_nutrients()</t>
+  </si>
+  <si>
+    <t>test_false_to_true_correctly_categorises_nutrients()</t>
+  </si>
+  <si>
+    <t>test_true_to_false_with_single_nutrient_correctly_categorises_opposing_implication()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -633,28 +642,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.26953125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" style="9" customWidth="1"/>
     <col min="7" max="7" width="25" style="9" customWidth="1"/>
-    <col min="8" max="8" width="95.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="125.28515625" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="3"/>
+    <col min="8" max="8" width="95.7265625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="125.26953125" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +692,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -712,7 +721,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>27</v>
       </c>
@@ -741,7 +750,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -770,7 +779,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -799,7 +808,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -828,7 +837,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -853,8 +862,11 @@
       <c r="H7" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -879,8 +891,11 @@
       <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -905,8 +920,11 @@
       <c r="H9" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -932,7 +950,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -958,7 +976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -984,7 +1002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1010,7 +1028,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -1036,7 +1054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1062,19 +1080,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I20" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Tests for _collects_nutrient_ratio_conflicts() all passing!
</commit_message>
<xml_diff>
--- a/docs/flag_conflict_logic_table~v2.xlsx
+++ b/docs/flag_conflict_logic_table~v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James.Izzard\Dropbox\pydiet\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.izzard\Dropbox\pydiet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91ACDEBC-87E7-42CC-B03F-2A463B987F18}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF38598-C1C4-4062-B201-83C9C8D5F3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="3210" windowWidth="43370" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26745" yWindow="3930" windowWidth="40515" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="44">
   <si>
     <t>Flag Type</t>
   </si>
@@ -107,9 +107,6 @@
     <t># Nutrients Matching False</t>
   </si>
   <si>
-    <t>Related nutrient in 'need_zero', 'need_non_zero'  to oppose implication.</t>
-  </si>
-  <si>
     <t>Zero or More</t>
   </si>
   <si>
@@ -143,7 +140,31 @@
     <t>test_false_to_true_correctly_categorises_nutrients()</t>
   </si>
   <si>
-    <t>test_true_to_false_with_single_nutrient_correctly_categorises_opposing_implication()</t>
+    <t>Direct Alias</t>
+  </si>
+  <si>
+    <t>Related nutrient in 'need_zero' or 'need_non_zero'  to oppose implication.</t>
+  </si>
+  <si>
+    <t>test_none_to_false_with_single_nutrient_correctly_categorises_opposing_implication()</t>
+  </si>
+  <si>
+    <t>test_true_to_none_with_direct_alias_single_nutrient_correctly_categorises_need_undefining()</t>
+  </si>
+  <si>
+    <t>test_true_to_false_with_direct_alias_single_nutrient_correctly_categorises_opposing_implication()</t>
+  </si>
+  <si>
+    <t>test_false_to_none_collects_all_defined_opposing_nutrients_in_need_undefining()</t>
+  </si>
+  <si>
+    <t>test_true_to_false_with_direct_alias_multiple_related_nutrients_collects_all_in_preventing_flag_false()</t>
+  </si>
+  <si>
+    <t>test_true_to_none_with_direct_alias_multiple_related_nutrients_collects_all_in_preventing_flag_undefine()</t>
+  </si>
+  <si>
+    <t>test_none_to_false_with_multiple_undefined_nutrients_collects_all_in_preventing_flag_false()</t>
   </si>
 </sst>
 </file>
@@ -269,7 +290,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -309,20 +330,6 @@
       <font>
         <color theme="0" tint="-0.34998626667073579"/>
       </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCC99FF"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -646,24 +653,24 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="17.54296875" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.26953125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="26.1796875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" style="9" customWidth="1"/>
     <col min="7" max="7" width="25" style="9" customWidth="1"/>
-    <col min="8" max="8" width="95.7265625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="125.26953125" style="12" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="3"/>
+    <col min="8" max="8" width="95.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="125.28515625" style="12" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,12 +696,12 @@
         <v>6</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>13</v>
@@ -703,27 +710,27 @@
         <v>13</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>13</v>
@@ -738,19 +745,19 @@
         <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
@@ -767,19 +774,19 @@
         <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -793,22 +800,22 @@
         <v>14</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -822,10 +829,10 @@
         <v>14</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>14</v>
@@ -834,10 +841,10 @@
         <v>9</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -851,10 +858,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>14</v>
@@ -863,10 +870,10 @@
         <v>16</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
@@ -880,24 +887,24 @@
         <v>14</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>19</v>
       </c>
       <c r="I8" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>1</v>
@@ -912,19 +919,19 @@
         <v>20</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -938,10 +945,10 @@
         <v>20</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>20</v>
@@ -949,10 +956,13 @@
       <c r="H10" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I10" s="12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>1</v>
@@ -967,16 +977,19 @@
         <v>20</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I11" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -990,21 +1003,24 @@
         <v>14</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I12" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>1</v>
@@ -1019,18 +1035,21 @@
         <v>14</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I13" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>1</v>
@@ -1045,16 +1064,19 @@
         <v>14</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I14" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
@@ -1068,31 +1090,34 @@
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I15" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I16" s="11"/>
     </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I17" s="11"/>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I20" s="11"/>
     </row>
   </sheetData>
@@ -1100,14 +1125,6 @@
     <sortCondition ref="D1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
-      <formula>"Has DOF"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="15" operator="equal">
-      <formula>"Direct Alias"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E15:G15 B2:G3 B1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>"N/A"</formula>

</xml_diff>

<commit_message>
- HasSettableFlags tests complete and passing.
</commit_message>
<xml_diff>
--- a/docs/flag_conflict_logic_table~v2.xlsx
+++ b/docs/flag_conflict_logic_table~v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.izzard\Dropbox\pydiet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF38598-C1C4-4062-B201-83C9C8D5F3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C34E8C-F2A9-4A01-81C2-14DD6E47FC75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26745" yWindow="3930" windowWidth="40515" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -653,7 +653,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1032,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>25</v>
@@ -1061,7 +1061,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F14" s="9" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Update HasNutrientRatios so .nutrient_ratios uses .get_nutrient_ratio.
Currently, the dependency is the other way around, which means we have to instantiate all of the nutrient ratios, just to get a single one.

This actually involved a reasonable overhaul of the HasSettableFlags tests, because by bad design, many of those were relying on the implementation of the .nutrient_ratios method. The nutrient ratio collection method is much more robustly tested after this work, because before and after tests were introduced to check that flag states were what they should have been, before the conflicts were collected.
</commit_message>
<xml_diff>
--- a/docs/flag_conflict_logic_table~v2.xlsx
+++ b/docs/flag_conflict_logic_table~v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.izzard\Dropbox\pydiet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C34E8C-F2A9-4A01-81C2-14DD6E47FC75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2EC68-C2BC-48AA-BCF7-DB489CAA3A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26745" yWindow="3930" windowWidth="40515" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34920" yWindow="4470" windowWidth="40515" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="46">
   <si>
     <t>Flag Type</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>test_none_to_false_with_multiple_undefined_nutrients_collects_all_in_preventing_flag_false()</t>
+  </si>
+  <si>
+    <t>test_none_to_false_with_dof_and_some_related_nutrients_collects_all_in_preventing_flag_false()</t>
+  </si>
+  <si>
+    <t>test_false_to_none_with_dof_and_some_related_nutrients_collects_all_in_preventing_flag_undefine()</t>
   </si>
 </sst>
 </file>
@@ -207,7 +213,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,6 +223,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -248,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -284,6 +296,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -650,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,7 +948,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>5</v>
@@ -962,60 +977,60 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>38</v>
+        <v>4</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1023,65 +1038,65 @@
         <v>35</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>2</v>
@@ -1090,42 +1105,100 @@
         <v>22</v>
       </c>
       <c r="E15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="9" t="s">
+      <c r="F17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="I17" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I16" s="11"/>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
-      <c r="I17" s="11"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I18" s="11"/>
     </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I20" s="11"/>
     </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" s="11"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:H20">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:H22">
     <sortCondition ref="D1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E15:G15 B2:G3 B1:D1048576">
+  <conditionalFormatting sqref="E17:G17 B2:G3 B1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -1136,7 +1209,7 @@
       <formula>"True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:D1048576 B1:D14">
+  <conditionalFormatting sqref="B27:D1048576 B1:D16">
     <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
       <formula>"None"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Tests the Ingredient class' concrete implementations of abstract methods.
These are the abstract methods required by the base classes, to allow the instance to access the information required for their specific functionality.
There are various tweaks to the test database, to make sure we have the correct characteristics to test in the saved ingredients.
</commit_message>
<xml_diff>
--- a/docs/flag_conflict_logic_table~v2.xlsx
+++ b/docs/flag_conflict_logic_table~v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.izzard\Dropbox\pydiet\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2EC68-C2BC-48AA-BCF7-DB489CAA3A84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1301E787-B6A1-4EB1-8635-4B8966E79AF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34920" yWindow="4470" windowWidth="40515" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37815" yWindow="5850" windowWidth="40080" windowHeight="14790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,159 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8F6FC4D6-2720-47B8-A3DB-CEAED3350BF7}</author>
+    <author>tc={648B532D-24E6-4E08-A69B-CB1E130133B5}</author>
+    <author>tc={09B4B6C6-3385-4D13-A362-8E82A04B2EE4}</author>
+    <author>tc={B6DE21D8-0D6D-4EB6-8C2A-40A8F72CBC62}</author>
+    <author>tc={C19E7007-4C24-4EB3-AD79-F9B48445EBE7}</author>
+    <author>tc={2D2DA5BD-631A-46B4-A31B-4016FB4A8018}</author>
+    <author>tc={372B50EF-FA14-43B4-8ED2-758528C99B00}</author>
+    <author>tc={3F64657E-A52C-4453-A22C-7799923DAA40}</author>
+    <author>tc={F3E68592-C3B6-4066-A9D5-BD13670DDE8B}</author>
+    <author>tc={D532384C-6272-416C-BFBF-DFB48234DFDB}</author>
+    <author>tc={26E9A4B7-1190-4565-99D6-637A5657B85C}</author>
+    <author>tc={27020A56-134A-4E23-83A9-9EB3EB765802}</author>
+    <author>tc={C6B90D63-A6A0-414D-B186-953791B795DA}</author>
+    <author>tc={755770FD-978F-4C96-9F07-EE58E2A28590}</author>
+    <author>tc={8C21564C-95DA-459B-8F77-592EBC74AF0C}</author>
+    <author>tc={5F6FA4CC-46D7-49F7-95A8-0BFCE4A7C2E2}</author>
+  </authors>
+  <commentList>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{8F6FC4D6-2720-47B8-A3DB-CEAED3350BF7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    If there are no related nutrients, the value of the flag depends entirely on the degree of freedom.</t>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="1" shapeId="0" xr:uid="{648B532D-24E6-4E08-A69B-CB1E130133B5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    If the flag has a degree of freedom, and all of the nutrients match True, then the degree of freedom is free to be set to anything.</t>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="2" shapeId="0" xr:uid="{09B4B6C6-3385-4D13-A362-8E82A04B2EE4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We are not changing the value here, so there should be no conflicts.</t>
+      </text>
+    </comment>
+    <comment ref="H5" authorId="3" shapeId="0" xr:uid="{B6DE21D8-0D6D-4EB6-8C2A-40A8F72CBC62}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We are not changing the value here, so there should be no conflicts.</t>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="4" shapeId="0" xr:uid="{C19E7007-4C24-4EB3-AD79-F9B48445EBE7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We are not changing the value here, so there should be no conflicts.</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="5" shapeId="0" xr:uid="{2D2DA5BD-631A-46B4-A31B-4016FB4A8018}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Since we only have one nutrient, we know exactly which one needs to be changed to oppose the flag implication.</t>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="6" shapeId="0" xr:uid="{372B50EF-FA14-43B4-8ED2-758528C99B00}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Since we have more than one nutrient, we can't tell which one(s) needs to be changed to oppose the flag impliciation.</t>
+      </text>
+    </comment>
+    <comment ref="H9" authorId="7" shapeId="0" xr:uid="{3F64657E-A52C-4453-A22C-7799923DAA40}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We only have one nutrient, so it must be that nutrient that needs to be undefined to make the flag undefined.</t>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="8" shapeId="0" xr:uid="{F3E68592-C3B6-4066-A9D5-BD13670DDE8B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We have more than one nutrient, so we don't know which one(s) we would have to undefine to make the flag undefined.</t>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="9" shapeId="0" xr:uid="{D532384C-6272-416C-BFBF-DFB48234DFDB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    To get a True result, every related nutrient needs to match its implication, so we can just sort them based on this.</t>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="10" shapeId="0" xr:uid="{26E9A4B7-1190-4565-99D6-637A5657B85C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Since we only have one nutrient, and the flag is a direct alias, we know it has to oppose the flags implication, so we can sort it.</t>
+      </text>
+    </comment>
+    <comment ref="H13" authorId="11" shapeId="0" xr:uid="{27020A56-134A-4E23-83A9-9EB3EB765802}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    We don't know which nutrient needs to be False to trigger the whole flag, so everything goes in 'preventing_flag_false'</t>
+      </text>
+    </comment>
+    <comment ref="H14" authorId="12" shapeId="0" xr:uid="{C6B90D63-A6A0-414D-B186-953791B795DA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is indetermiant. We don't know whether  all of the related nutrients need to match the flag so the DOF is free to drive the value, or wether one or more of the nutrients need to be set to oppose the flag.</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="13" shapeId="0" xr:uid="{755770FD-978F-4C96-9F07-EE58E2A28590}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Easy, we are changing to True, so we just need all the nutrients to match thier implications. We sort them based on this.</t>
+      </text>
+    </comment>
+    <comment ref="H16" authorId="14" shapeId="0" xr:uid="{8C21564C-95DA-459B-8F77-592EBC74AF0C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Since an opposing nutrient will always cause a False flag, even if other nutrients are undefined, we simply need to undefine all opposing nutrients.</t>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="15" shapeId="0" xr:uid="{5F6FA4CC-46D7-49F7-95A8-0BFCE4A7C2E2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This is indeterminate. We don't know wether we need to get all the nutrients to match the flag and use the DOF to undefine it, or undefine the nutrients currently causing False.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="46">
   <si>
@@ -146,18 +299,12 @@
     <t>Related nutrient in 'need_zero' or 'need_non_zero'  to oppose implication.</t>
   </si>
   <si>
-    <t>test_none_to_false_with_single_nutrient_correctly_categorises_opposing_implication()</t>
-  </si>
-  <si>
     <t>test_true_to_none_with_direct_alias_single_nutrient_correctly_categorises_need_undefining()</t>
   </si>
   <si>
     <t>test_true_to_false_with_direct_alias_single_nutrient_correctly_categorises_opposing_implication()</t>
   </si>
   <si>
-    <t>test_false_to_none_collects_all_defined_opposing_nutrients_in_need_undefining()</t>
-  </si>
-  <si>
     <t>test_true_to_false_with_direct_alias_multiple_related_nutrients_collects_all_in_preventing_flag_false()</t>
   </si>
   <si>
@@ -167,17 +314,23 @@
     <t>test_none_to_false_with_multiple_undefined_nutrients_collects_all_in_preventing_flag_false()</t>
   </si>
   <si>
-    <t>test_none_to_false_with_dof_and_some_related_nutrients_collects_all_in_preventing_flag_false()</t>
-  </si>
-  <si>
-    <t>test_false_to_none_with_dof_and_some_related_nutrients_collects_all_in_preventing_flag_undefine()</t>
+    <t>test_none_to_false_with_dof_collects_all_in_preventing_flag_false()</t>
+  </si>
+  <si>
+    <t>test_false_to_none_with_dof_collects_all_in_preventing_flag_undefine()</t>
+  </si>
+  <si>
+    <t>test_false_to_none_with_direct_alias_collects_all_defined_opposing_nutrients_in_need_undefining()</t>
+  </si>
+  <si>
+    <t>test_none_to_false_with_direct_alias_single_nutrient_correctly_categorises_opposing_implication()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,8 +365,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,12 +382,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,7 +451,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -366,6 +519,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="James Izzard" id="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" userId="S::James.Izzard@ttp.com::8815d481-cb8b-4531-b6fb-d20944c0b0bc" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -663,12 +822,65 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H2" dT="2021-05-22T18:44:11.66" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{8F6FC4D6-2720-47B8-A3DB-CEAED3350BF7}">
+    <text>If there are no related nutrients, the value of the flag depends entirely on the degree of freedom.</text>
+  </threadedComment>
+  <threadedComment ref="H3" dT="2021-05-22T18:44:51.00" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{648B532D-24E6-4E08-A69B-CB1E130133B5}">
+    <text>If the flag has a degree of freedom, and all of the nutrients match True, then the degree of freedom is free to be set to anything.</text>
+  </threadedComment>
+  <threadedComment ref="H4" dT="2021-05-22T18:45:55.73" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{09B4B6C6-3385-4D13-A362-8E82A04B2EE4}">
+    <text>We are not changing the value here, so there should be no conflicts.</text>
+  </threadedComment>
+  <threadedComment ref="H5" dT="2021-05-22T18:46:10.29" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{B6DE21D8-0D6D-4EB6-8C2A-40A8F72CBC62}">
+    <text>We are not changing the value here, so there should be no conflicts.</text>
+  </threadedComment>
+  <threadedComment ref="H6" dT="2021-05-22T18:46:16.50" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{C19E7007-4C24-4EB3-AD79-F9B48445EBE7}">
+    <text>We are not changing the value here, so there should be no conflicts.</text>
+  </threadedComment>
+  <threadedComment ref="H7" dT="2021-05-22T18:49:42.30" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{2D2DA5BD-631A-46B4-A31B-4016FB4A8018}">
+    <text>Since we only have one nutrient, we know exactly which one needs to be changed to oppose the flag implication.</text>
+  </threadedComment>
+  <threadedComment ref="H8" dT="2021-05-22T18:50:26.86" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{372B50EF-FA14-43B4-8ED2-758528C99B00}">
+    <text>Since we have more than one nutrient, we can't tell which one(s) needs to be changed to oppose the flag impliciation.</text>
+  </threadedComment>
+  <threadedComment ref="H9" dT="2021-05-22T18:51:49.36" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{3F64657E-A52C-4453-A22C-7799923DAA40}">
+    <text>We only have one nutrient, so it must be that nutrient that needs to be undefined to make the flag undefined.</text>
+  </threadedComment>
+  <threadedComment ref="H10" dT="2021-05-22T18:52:20.58" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{F3E68592-C3B6-4066-A9D5-BD13670DDE8B}">
+    <text>We have more than one nutrient, so we don't know which one(s) we would have to undefine to make the flag undefined.</text>
+  </threadedComment>
+  <threadedComment ref="H11" dT="2021-05-22T18:54:29.39" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{D532384C-6272-416C-BFBF-DFB48234DFDB}">
+    <text>To get a True result, every related nutrient needs to match its implication, so we can just sort them based on this.</text>
+  </threadedComment>
+  <threadedComment ref="H12" dT="2021-05-22T18:57:54.88" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{26E9A4B7-1190-4565-99D6-637A5657B85C}">
+    <text>Since we only have one nutrient, and the flag is a direct alias, we know it has to oppose the flags implication, so we can sort it.</text>
+  </threadedComment>
+  <threadedComment ref="H13" dT="2021-05-22T17:48:51.60" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{27020A56-134A-4E23-83A9-9EB3EB765802}">
+    <text>We don't know which nutrient needs to be False to trigger the whole flag, so everything goes in 'preventing_flag_false'</text>
+  </threadedComment>
+  <threadedComment ref="H14" dT="2021-05-22T19:01:03.98" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{C6B90D63-A6A0-414D-B186-953791B795DA}">
+    <text>This is indetermiant. We don't know whether  all of the related nutrients need to match the flag so the DOF is free to drive the value, or wether one or more of the nutrients need to be set to oppose the flag.</text>
+  </threadedComment>
+  <threadedComment ref="H15" dT="2021-05-22T18:56:25.34" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{755770FD-978F-4C96-9F07-EE58E2A28590}">
+    <text>Easy, we are changing to True, so we just need all the nutrients to match thier implications. We sort them based on this.</text>
+  </threadedComment>
+  <threadedComment ref="H16" dT="2021-05-22T19:03:53.60" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{8C21564C-95DA-459B-8F77-592EBC74AF0C}">
+    <text>Since an opposing nutrient will always cause a False flag, even if other nutrients are undefined, we simply need to undefine all opposing nutrients.</text>
+  </threadedComment>
+  <threadedComment ref="H17" dT="2021-05-22T19:05:27.13" personId="{437548AB-E34F-4DB6-A9BE-79A598C8CE30}" id="{5F6FA4CC-46D7-49F7-95A8-0BFCE4A7C2E2}">
+    <text>This is indeterminate. We don't know wether we need to get all the nutrients to match the flag and use the DOF to undefine it, or undefine the nutrients currently causing False.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,60 +1073,60 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>1</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -925,7 +1137,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>20</v>
@@ -939,11 +1151,11 @@
       <c r="G9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="6" t="s">
-        <v>36</v>
+      <c r="H9" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -951,39 +1163,39 @@
         <v>35</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>14</v>
@@ -998,10 +1210,10 @@
         <v>14</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1009,28 +1221,28 @@
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>25</v>
-      </c>
       <c r="H12" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1038,28 +1250,28 @@
         <v>35</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>5</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1067,10 +1279,10 @@
         <v>26</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>2</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>14</v>
@@ -1079,45 +1291,45 @@
         <v>24</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>45</v>
+        <v>4</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="D15" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1125,56 +1337,56 @@
         <v>35</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="I16" s="12" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B17" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>2</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1194,11 +1406,11 @@
       <c r="I22" s="11"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:H22">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A16:H22">
     <sortCondition ref="D1"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="E17:G17 B2:G3 B1:D1048576">
+  <conditionalFormatting sqref="E13:G13 B2:G3 B1:D1048576">
     <cfRule type="cellIs" dxfId="5" priority="10" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
@@ -1209,7 +1421,7 @@
       <formula>"True"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:D1048576 B1:D16">
+  <conditionalFormatting sqref="B27:D1048576 B1:D17">
     <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
       <formula>"None"</formula>
     </cfRule>
@@ -1224,5 +1436,6 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>